<commit_message>
Auto-committed on 2023/09/15 週五 11:49:41.89
</commit_message>
<xml_diff>
--- a/Program/Other/LM073_底稿_央行報送明細資料.xlsx
+++ b/Program/Other/LM073_底稿_央行報送明細資料.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6B6E53-4AEA-4EED-936D-C668AF0D95D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCF44D6-FFD5-42C3-A986-A18D99B268CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="明細" sheetId="9" r:id="rId1"/>
@@ -23,38 +23,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>戶號</t>
+  </si>
+  <si>
+    <t>額度</t>
+  </si>
+  <si>
+    <t>首次撥款日</t>
+  </si>
+  <si>
+    <t>核准額度</t>
+  </si>
+  <si>
+    <t>撥款日期</t>
+  </si>
+  <si>
+    <t>撥款金額</t>
+  </si>
   <si>
     <t>地區別</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>規定管制代碼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶號</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>額度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>核准額度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>核准利率%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>鑑估總值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初貸日</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>撥款</t>
+  </si>
+  <si>
+    <t>利率</t>
+  </si>
+  <si>
+    <t>貸款成數</t>
+  </si>
+  <si>
+    <t>評估淨值</t>
+  </si>
+  <si>
+    <t>代償碼</t>
+  </si>
+  <si>
+    <t>展期/借新還舊</t>
   </si>
 </sst>
 </file>
@@ -713,14 +720,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -791,9 +795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -831,9 +835,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -866,26 +870,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -918,26 +905,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1111,56 +1081,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7A4DF7-0CF1-41DB-9838-6118AECA276A}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.90625" style="1"/>
+    <col min="13" max="13" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/21 週四 11:45:41.07
</commit_message>
<xml_diff>
--- a/Program/Other/LM073_底稿_央行報送明細資料.xlsx
+++ b/Program/Other/LM073_底稿_央行報送明細資料.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCF44D6-FFD5-42C3-A986-A18D99B268CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D9C686-5CCE-4704-B44E-28C0BB49F778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>戶號</t>
   </si>
@@ -62,6 +62,10 @@
   </si>
   <si>
     <t>展期/借新還舊</t>
+  </si>
+  <si>
+    <t>央管代碼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -431,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -591,6 +595,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -720,7 +750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,6 +765,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1081,71 +1117,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7A4DF7-0CF1-41DB-9838-6118AECA276A}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.90625" style="1"/>
-    <col min="13" max="13" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="3" width="12.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.90625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" style="1"/>
+    <col min="15" max="15" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>